<commit_message>
Adding MPA test automation upload file
</commit_message>
<xml_diff>
--- a/01_change_upload.xlsx
+++ b/01_change_upload.xlsx
@@ -3524,7 +3524,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20000057</t>
+          <t>20000058</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>60000152</t>
+          <t>60000165</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3835,7 +3835,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -3987,7 +3987,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>60000153</t>
+          <t>60000166</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>124</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4293,7 +4293,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>60000154</t>
+          <t>60000167</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">

</xml_diff>